<commit_message>
Them man hinh them/sua mon an, Thay doi trang thai mon an, Them man hinh Bao cao Doanh Thu(Chua ket noi database)
</commit_message>
<xml_diff>
--- a/build/classes/ExportFile_Excel/DanhsachHoaDon_26-05-2023.xlsx
+++ b/build/classes/ExportFile_Excel/DanhsachHoaDon_26-05-2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>none</t>
   </si>
@@ -38,30 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tổng tiền</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>23-05-2023</t>
-  </si>
-  <si>
-    <t>779,000đ</t>
-  </si>
-  <si>
-    <t>0đ</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>25-05-2023</t>
-  </si>
-  <si>
-    <t>6,070,000đ</t>
   </si>
 </sst>
 </file>
@@ -373,7 +349,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,7 +361,7 @@
     <col min="4" max="4" width="15.286830357142858" style="0" customWidth="1"/>
     <col min="5" max="5" width="13.286830357142858" style="0" customWidth="1"/>
     <col min="6" max="6" width="10.4296875" style="0" customWidth="1"/>
-    <col min="7" max="7" width="12.858258928571429" style="0" customWidth="1"/>
+    <col min="7" max="7" width="10.286830357142858" style="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0">
@@ -409,52 +385,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" ht="15.0">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" ht="15.0">
-      <c r="A3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>